<commit_message>
Update audit variables codebook.xlsx
update codebook
</commit_message>
<xml_diff>
--- a/audit variables codebook.xlsx
+++ b/audit variables codebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\labor_audit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cdocuments\GitHub\labor_audit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C16DA75-B596-4986-AC1F-9EAB6A25F46D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064FAF28-731B-4AB0-B555-380EA41F63BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="17115" windowHeight="10755" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="16395" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="code book" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="161">
   <si>
     <t>Variable name</t>
   </si>
@@ -91,12 +91,6 @@
     <t>the presence of workplace union =1</t>
   </si>
   <si>
-    <t>mng</t>
-  </si>
-  <si>
-    <t>management system: the average of 0 vs. 1 answers to 3 questions on human resources management and health &amp; safety management practices</t>
-  </si>
-  <si>
     <t>YearOperate</t>
   </si>
   <si>
@@ -437,9 +431,6 @@
   </si>
   <si>
     <t>buyer3FTindex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FTI ranked 150 fashion brands in 2018. But our data has 870 unique buyer names in total and 371 names for the first buyer. </t>
   </si>
   <si>
     <t>definition or operation</t>
@@ -447,17 +438,92 @@
   <si>
     <t>Is there an adequate accident investigation procedure?</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mngindex13</t>
+  </si>
+  <si>
+    <t>the index of management system considering audits that included all 13 items</t>
+  </si>
+  <si>
+    <t>mngpc</t>
+  </si>
+  <si>
+    <t>the percentage of implemented management system items among total items (ranging from 10 to 13 total items)</t>
+  </si>
+  <si>
+    <t>buyer1FTindexband</t>
+  </si>
+  <si>
+    <t>buyer2FTindexband</t>
+  </si>
+  <si>
+    <t>buyer3FTindexband</t>
+  </si>
+  <si>
+    <t>these are percentage points out of a total of 250 points, ranging from 0 to 100 theorectically and from 0 to 58 for buyer 1.</t>
+  </si>
+  <si>
+    <t>recode buyer1 Fashion transparency index into ordinal categories based on Fashion Transparency's scale: 1 for 1-10, 2 for 11 to 20; 3 for 21-30, 4 for 31 to 40, 5 for 41 to 50, 6 for 51 to 60 etc.</t>
+  </si>
+  <si>
+    <t>recode buyer2 Fashion transparency index into ordinal categories based on Fashion Transparency's scale: 1 for 1-10, 2 for 11 to 20; 3 for 21-30, 4 for 31 to 40, 5 for 41 to 50, 6 for 51 to 60 etc.</t>
+  </si>
+  <si>
+    <t>recode buyer3 Fashion transparency index into ordinal categories based on Fashion Transparency's scale: 1 for 1-10, 2 for 11 to 20; 3 for 21-30, 4 for 31 to 40, 5 for 41 to 50, 6 for 51 to 60 etc.</t>
+  </si>
+  <si>
+    <t>Note that the -1 (unrated and -2 (missing buyer names) are both coded into 0 since they may belong to the same band of firms under the radiar.</t>
+  </si>
+  <si>
+    <t>RRic3yr</t>
+  </si>
+  <si>
+    <t>RRic5yr</t>
+  </si>
+  <si>
+    <t>RRic2010</t>
+  </si>
+  <si>
+    <t>RepRiskID</t>
+  </si>
+  <si>
+    <t>the factory's ID in RepRisk dataset which collect labor/environemental violations news across the world</t>
+  </si>
+  <si>
+    <t>the presence of workplace union =1 for each audit/year</t>
+  </si>
+  <si>
+    <t>some factories changed union status across the years</t>
+  </si>
+  <si>
+    <t>count the number of labor/environmental rights abuse news collected by RepRisk dataset in the previous three years before the audit date.</t>
+  </si>
+  <si>
+    <t>count the number of labor/environmental rights abuse news collected by RepRisk dataset in the previous five years before the audit date.</t>
+  </si>
+  <si>
+    <t>count the number of labor/environmental rights abuse news collected by RepRisk dataset from 2010 January to the audit date.</t>
+  </si>
+  <si>
+    <t>Those factory names that did not show up in RepRisk dataset as well as those that showed up but did not have any news incidents were both coded as 0. There are 430 obsers larger than 0 ( a lot of 0s)</t>
+  </si>
+  <si>
+    <t>Those factory names that did not show up in RepRisk dataset as well as those that showed up but did not have any news incidents were both coded as 0. There are 583 obs larger than 0.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Those factory names that did not show up in RepRisk dataset as well as those that showed up but did not have any news incidents were both coded as 0. There are 712 obs larger than 0. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -465,22 +531,36 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -510,13 +590,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,15 +879,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="1" max="1" width="16.46484375" customWidth="1"/>
     <col min="2" max="2" width="77.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -814,7 +896,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -886,7 +968,7 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -963,7 +1045,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
         <v>37</v>
@@ -971,10 +1053,10 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
         <v>40</v>
-      </c>
-      <c r="B21" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1097,11 +1179,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
         <v>71</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1121,39 +1203,137 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
-        <v>77</v>
-      </c>
-      <c r="B41" t="s">
-        <v>78</v>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>128</v>
+      </c>
+      <c r="B42" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B43" t="s">
-        <v>132</v>
-      </c>
-      <c r="C43" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B44" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
-        <v>135</v>
-      </c>
-      <c r="B45" t="s">
-        <v>134</v>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1167,11 +1347,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055C5207-483C-47F2-9B33-4BD985FA48B1}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="14.9296875" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
@@ -1182,202 +1362,202 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="B1" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
         <v>79</v>
       </c>
-      <c r="B2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" t="s">
-        <v>81</v>
-      </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="3"/>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="3"/>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="3"/>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="3"/>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="3"/>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="3"/>
       <c r="B9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="3"/>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="3"/>
       <c r="B11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C11" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="3"/>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="3"/>
       <c r="B13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="3"/>
       <c r="B14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="B16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="2:3">
       <c r="B17" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
0830 transparency sub coding
update codebook about coding subelements of transparency index
</commit_message>
<xml_diff>
--- a/audit variables codebook.xlsx
+++ b/audit variables codebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cdocuments\GitHub\labor_audit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B764425-6BAB-48DA-BD6F-C7113E028F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4563719A-350D-421D-AEDD-73C6A38377DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="16395" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="203">
   <si>
     <t>Variable name</t>
   </si>
@@ -537,6 +537,108 @@
   </si>
   <si>
     <t xml:space="preserve">count the number of labor/environment rights abuse news collected by Reprisk dataset between audits (e.g between the 2nd and 3rd AssessmentDate); for the first audit for a particular factory, count the number of news from 2010. </t>
+  </si>
+  <si>
+    <t>buyer1pol18</t>
+  </si>
+  <si>
+    <t>buyer1gov19</t>
+  </si>
+  <si>
+    <t>buyer1trace18</t>
+  </si>
+  <si>
+    <t>buyer1gov18</t>
+  </si>
+  <si>
+    <t>buyer2trace18</t>
+  </si>
+  <si>
+    <t>buyer3trace18</t>
+  </si>
+  <si>
+    <t>buyertracemx18</t>
+  </si>
+  <si>
+    <t>buyer1know18</t>
+  </si>
+  <si>
+    <t>buyer2know18</t>
+  </si>
+  <si>
+    <t>buyer3know18</t>
+  </si>
+  <si>
+    <t>buyerknowmx18</t>
+  </si>
+  <si>
+    <t>buyer1pol19</t>
+  </si>
+  <si>
+    <t>buyer1trace19</t>
+  </si>
+  <si>
+    <t>buyer2trace19</t>
+  </si>
+  <si>
+    <t>buyer3trace19</t>
+  </si>
+  <si>
+    <t>buyertracemx19</t>
+  </si>
+  <si>
+    <t>buyer1know19</t>
+  </si>
+  <si>
+    <t>buyer2know19</t>
+  </si>
+  <si>
+    <t>buyer3know19</t>
+  </si>
+  <si>
+    <t>buyerknowmx19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Values: 0=unrated or missing buyer names; 1 for index score between 0-10%, 2 for 11-20, 3 for 21-30, 4 for 31-40, 5 for 41-50, 6 for 51-60, 7 for 61-70, 8 for 71-80, 9 for 81-90, 10 for 91-100. </t>
+  </si>
+  <si>
+    <t>the maximum traceability index among the three buyers in 2018</t>
+  </si>
+  <si>
+    <t>the first buyer's transparency index regarding "policy and commitment" in 2018.</t>
+  </si>
+  <si>
+    <t>the first buyer's transparency index regarding "governance" in 2018.</t>
+  </si>
+  <si>
+    <t>the first buyer's transparency index regarding "traceability" in 2018.</t>
+  </si>
+  <si>
+    <t>the second buyer's transparency index regarding "traceability" in 2018.</t>
+  </si>
+  <si>
+    <t>the third buyer's transparency index regarding "traceability" in 2018.</t>
+  </si>
+  <si>
+    <t>the first buyer's transparency index regarding "know/audit, show, and fix" in 2018</t>
+  </si>
+  <si>
+    <t>the second buyer's transparency index regarding "know/audit, show, and fix" in 2018</t>
+  </si>
+  <si>
+    <t>the third buyer's transparency index regarding "know/audit, show, and fix" in 2018</t>
+  </si>
+  <si>
+    <t>the biggest "know/audit, show, and fix" index among three buyers in 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">values: same as above </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the same set of variables and coding for the transparency index report in 2019 (which included 50 more brands). </t>
+  </si>
+  <si>
+    <t>definition is the same as 2018</t>
   </si>
 </sst>
 </file>
@@ -903,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1171,7 +1273,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -1179,7 +1281,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>65</v>
       </c>
@@ -1187,7 +1289,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>67</v>
       </c>
@@ -1195,7 +1297,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>69</v>
       </c>
@@ -1203,7 +1305,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>71</v>
       </c>
@@ -1211,7 +1313,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:2">
       <c r="A39" s="3" t="s">
         <v>165</v>
       </c>
@@ -1219,7 +1321,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>73</v>
       </c>
@@ -1227,91 +1329,13 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>75</v>
       </c>
       <c r="B41" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
-        <v>128</v>
-      </c>
-      <c r="B43" t="s">
-        <v>130</v>
-      </c>
-      <c r="C43" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
-        <v>129</v>
-      </c>
-      <c r="B44" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
-        <v>133</v>
-      </c>
-      <c r="B45" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C50" s="3"/>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C51" s="3"/>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="3"/>
@@ -1393,6 +1417,266 @@
       <c r="C62" s="3" t="s">
         <v>154</v>
       </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>128</v>
+      </c>
+      <c r="B66" t="s">
+        <v>130</v>
+      </c>
+      <c r="C66" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>129</v>
+      </c>
+      <c r="B67" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>133</v>
+      </c>
+      <c r="B68" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C73" s="3"/>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C74" s="3"/>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C77" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C78" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C79" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C80" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C81" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C82" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C83" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C84" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C85" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C86" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="2"/>
+      <c r="B87" s="2"/>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B88" s="2"/>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B90" s="2"/>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B91" s="2"/>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B92" s="2"/>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B93" s="2"/>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B94" s="2"/>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B95" s="2"/>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B96" s="2"/>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B97" s="2"/>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B98" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>